<commit_message>
Implemented LinearSVM for method 1, and trained the classifier.
</commit_message>
<xml_diff>
--- a/Classifier Metrics.xlsx
+++ b/Classifier Metrics.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="141" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="284" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,9 +15,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
-  <si>
-    <t>Classifier </t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+  <si>
+    <t>Classifier</t>
   </si>
   <si>
     <t>Time to Train in Min</t>
@@ -66,6 +66,9 @@
   </si>
   <si>
     <t>Ada Boost</t>
+  </si>
+  <si>
+    <t>Linear SVM</t>
   </si>
   <si>
     <t>Trained over:</t>
@@ -95,6 +98,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -117,6 +121,7 @@
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -282,8 +287,8 @@
   </sheetPr>
   <dimension ref="B3:J29"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H26" activeCellId="0" sqref="H26"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J12" activeCellId="0" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.7"/>
@@ -560,16 +565,34 @@
         <v>0.566</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="13.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="5"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
+    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="4" t="n">
+        <v>27.4154318174</v>
+      </c>
+      <c r="D12" s="4" t="n">
+        <v>0.5965</v>
+      </c>
+      <c r="E12" s="4" t="n">
+        <v>0.608822103732</v>
+      </c>
+      <c r="F12" s="4" t="n">
+        <v>0.583376355188</v>
+      </c>
+      <c r="G12" s="4" t="n">
+        <v>0.590780809031</v>
+      </c>
+      <c r="H12" s="4" t="n">
+        <v>0.602988260406</v>
+      </c>
+      <c r="I12" s="4" t="n">
+        <v>0.628</v>
+      </c>
+      <c r="J12" s="4" t="n">
+        <v>0.565</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="13.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="4"/>
@@ -583,19 +606,19 @@
     </row>
     <row r="17" customFormat="false" ht="13.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>